<commit_message>
Adjustment Phase 0 - all docs updated - need to merge back to stable - few manual test to be updated - random checks
</commit_message>
<xml_diff>
--- a/00_nightly_only/rhub.xlsx
+++ b/00_nightly_only/rhub.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igayen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igayen\Documents\RBI\WorkSpace\R_Packages\Nightly\tidycells_nightly\00_nightly_only\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6315"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6315" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="112">
   <si>
     <t>OS</t>
   </si>
@@ -344,6 +344,24 @@
   </si>
   <si>
     <t>read xls (preferred option)</t>
+  </si>
+  <si>
+    <t>tidycells::collate_columns --&gt; tidycells:::similarity_score</t>
+  </si>
+  <si>
+    <t>stringdist</t>
+  </si>
+  <si>
+    <t>stats</t>
+  </si>
+  <si>
+    <t>tidycells::collate_columns --&gt; tidycells:::similarity_score (Enhance)</t>
+  </si>
+  <si>
+    <t>**Imports**</t>
+  </si>
+  <si>
+    <t>**Suggests**</t>
   </si>
 </sst>
 </file>
@@ -439,12 +457,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -455,6 +472,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,437 +1086,485 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="A13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="5" t="s">
+    <row r="19" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5" t="s">
-        <v>90</v>
-      </c>
+    <row r="25" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>98</v>
-      </c>
+    <row r="27" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="2"/>
+    <row r="35" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="7"/>
     </row>
   </sheetData>
+  <sortState ref="A2:E31">
+    <sortCondition ref="B2:B31"/>
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1505,435 +1580,435 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6" t="s">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>